<commit_message>
Fixed data issues with card files.
</commit_message>
<xml_diff>
--- a/REFERENCES/Cards_Planning/Cards_Detailed.xlsx
+++ b/REFERENCES/Cards_Planning/Cards_Detailed.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\altam\OneDrive\Documents\GIT\MechsAndMagesPrototype\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\altam\OneDrive\Documents\GIT\MechsAndMagesPrototype\REFERENCES\Cards_Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:101_{8857B79B-5EEF-43FF-A0AA-0D696C79545D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90622BD1-815A-4295-A775-41B2CD386D9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="74">
   <si>
     <t>Quantity</t>
   </si>
@@ -141,9 +141,6 @@
   </si>
   <si>
     <t>#18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Heal </t>
   </si>
   <si>
     <t>#19</t>
@@ -945,7 +942,6 @@
             </c:spPr>
           </c:marker>
           <c:trendline>
-            <c:name/>
             <c:spPr>
               <a:ln w="19050" cap="rnd">
                 <a:solidFill>
@@ -1112,7 +1108,6 @@
             </c:spPr>
           </c:marker>
           <c:trendline>
-            <c:name/>
             <c:spPr>
               <a:ln w="19050" cap="rnd">
                 <a:solidFill>
@@ -1267,7 +1262,6 @@
             </c:spPr>
           </c:marker>
           <c:trendline>
-            <c:name/>
             <c:spPr>
               <a:ln w="19050" cap="rnd">
                 <a:solidFill>
@@ -1452,7 +1446,6 @@
             </c:extLst>
           </c:dPt>
           <c:trendline>
-            <c:name/>
             <c:spPr>
               <a:ln w="19050" cap="rnd">
                 <a:solidFill>
@@ -1607,7 +1600,6 @@
             </c:spPr>
           </c:marker>
           <c:trendline>
-            <c:name/>
             <c:spPr>
               <a:ln w="19050" cap="rnd">
                 <a:solidFill>
@@ -2966,7 +2958,7 @@
   <dimension ref="A1:AE51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AD55" sqref="AD55"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3041,7 +3033,7 @@
         <v>1</v>
       </c>
       <c r="AC2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AD2">
         <v>0</v>
@@ -3087,7 +3079,7 @@
         <v>1</v>
       </c>
       <c r="AC3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AD3">
         <v>25</v>
@@ -3120,11 +3112,11 @@
         <v>2</v>
       </c>
       <c r="J4">
-        <f t="shared" ref="J3:J33" si="0">E4+F4</f>
+        <f t="shared" ref="J4:J27" si="0">E4+F4</f>
         <v>1</v>
       </c>
       <c r="K4">
-        <f t="shared" ref="K3:K51" si="1">G4+I4</f>
+        <f t="shared" ref="K4:K39" si="1">G4+I4</f>
         <v>2</v>
       </c>
     </row>
@@ -3648,7 +3640,7 @@
         <v>4</v>
       </c>
       <c r="H19" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="I19">
         <v>2</v>
@@ -3667,7 +3659,7 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C20" t="str">
         <f t="shared" si="2"/>
@@ -3699,7 +3691,7 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C21" t="str">
         <f t="shared" si="2"/>
@@ -3737,7 +3729,7 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C22" t="str">
         <f t="shared" si="2"/>
@@ -3775,7 +3767,7 @@
         <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C23" t="str">
         <f t="shared" si="2"/>
@@ -3813,7 +3805,7 @@
         <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C24" t="str">
         <f t="shared" si="2"/>
@@ -3845,7 +3837,7 @@
         <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C25" t="str">
         <f t="shared" si="2"/>
@@ -3864,7 +3856,7 @@
         <v>4</v>
       </c>
       <c r="H25" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="I25">
         <v>3</v>
@@ -3883,7 +3875,7 @@
         <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C26" t="str">
         <f t="shared" si="2"/>
@@ -3921,7 +3913,7 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C27" t="str">
         <f t="shared" si="2"/>
@@ -3959,14 +3951,14 @@
         <v>1</v>
       </c>
       <c r="B28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C28" t="str">
         <f t="shared" si="2"/>
         <v>Green#27</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E28">
         <v>7</v>
@@ -3978,11 +3970,11 @@
         <v>9</v>
       </c>
       <c r="J28">
-        <f>E28+F28</f>
+        <f t="shared" ref="J28:J37" si="3">E28+F28</f>
         <v>9</v>
       </c>
       <c r="K28">
-        <f>G28+I28</f>
+        <f t="shared" ref="K28:K37" si="4">G28+I28</f>
         <v>9</v>
       </c>
     </row>
@@ -3991,14 +3983,14 @@
         <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C29" t="str">
         <f t="shared" si="2"/>
         <v>Green#28</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E29">
         <v>9</v>
@@ -4010,11 +4002,11 @@
         <v>11</v>
       </c>
       <c r="J29">
-        <f>E29+F29</f>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="K29">
-        <f>G29+I29</f>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
     </row>
@@ -4023,14 +4015,14 @@
         <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C30" t="str">
         <f t="shared" si="2"/>
         <v>Green#29</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E30">
         <v>7</v>
@@ -4042,11 +4034,11 @@
         <v>11</v>
       </c>
       <c r="J30">
-        <f>E30+F30</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="K30">
-        <f>G30+I30</f>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
     </row>
@@ -4055,14 +4047,14 @@
         <v>1</v>
       </c>
       <c r="B31" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C31" t="str">
         <f t="shared" si="2"/>
         <v>Green#30</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E31">
         <v>9</v>
@@ -4074,11 +4066,11 @@
         <v>13</v>
       </c>
       <c r="J31">
-        <f>E31+F31</f>
+        <f t="shared" si="3"/>
         <v>13</v>
       </c>
       <c r="K31">
-        <f>G31+I31</f>
+        <f t="shared" si="4"/>
         <v>13</v>
       </c>
     </row>
@@ -4087,14 +4079,14 @@
         <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C32" t="str">
         <f t="shared" si="2"/>
         <v>Green#31</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E32">
         <v>11</v>
@@ -4106,17 +4098,17 @@
         <v>12</v>
       </c>
       <c r="H32" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I32">
         <v>2</v>
       </c>
       <c r="J32">
-        <f>E32+F32</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="K32">
-        <f>G32+I32</f>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
     </row>
@@ -4125,14 +4117,14 @@
         <v>1</v>
       </c>
       <c r="B33" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C33" t="str">
         <f t="shared" si="2"/>
         <v>Green#32</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E33">
         <v>11</v>
@@ -4144,11 +4136,11 @@
         <v>14</v>
       </c>
       <c r="J33">
-        <f>E33+F33</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="K33">
-        <f>G33+I33</f>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
     </row>
@@ -4157,33 +4149,36 @@
         <v>1</v>
       </c>
       <c r="B34" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C34" t="str">
         <f t="shared" si="2"/>
         <v>Green#33</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E34">
         <v>12</v>
       </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
       <c r="G34">
         <v>14</v>
       </c>
       <c r="H34" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I34">
         <v>2</v>
       </c>
       <c r="J34">
-        <f>E34+F34</f>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="K34">
-        <f>G34+I34</f>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
     </row>
@@ -4192,27 +4187,30 @@
         <v>1</v>
       </c>
       <c r="B35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C35" t="str">
         <f t="shared" si="2"/>
         <v>Green#34</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E35">
         <v>12</v>
       </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
       <c r="G35">
         <v>15</v>
       </c>
       <c r="J35">
-        <f>E35+F35</f>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="K35">
-        <f>G35+I35</f>
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
     </row>
@@ -4221,33 +4219,36 @@
         <v>1</v>
       </c>
       <c r="B36" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C36" t="str">
         <f t="shared" si="2"/>
         <v>Green#35</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E36">
         <v>14</v>
       </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
       <c r="G36">
         <v>17</v>
       </c>
       <c r="H36" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I36">
         <v>1</v>
       </c>
       <c r="J36">
-        <f>E36+F36</f>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="K36">
-        <f>G36+I36</f>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
     </row>
@@ -4256,14 +4257,14 @@
         <v>1</v>
       </c>
       <c r="B37" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C37" t="str">
         <f t="shared" si="2"/>
         <v>Green#36</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E37">
         <v>15</v>
@@ -4275,17 +4276,17 @@
         <v>19</v>
       </c>
       <c r="H37" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I37">
         <v>2</v>
       </c>
       <c r="J37">
-        <f>E37+F37</f>
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
       <c r="K37">
-        <f>G37+I37</f>
+        <f t="shared" si="4"/>
         <v>21</v>
       </c>
     </row>
@@ -4294,14 +4295,14 @@
         <v>1</v>
       </c>
       <c r="B38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C38" t="str">
         <f t="shared" si="2"/>
         <v>Green#37</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E38">
         <v>15</v>
@@ -4313,13 +4314,13 @@
         <v>17</v>
       </c>
       <c r="H38" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I38">
         <v>2</v>
       </c>
       <c r="J38">
-        <f t="shared" ref="J35:J51" si="3">E38+F38</f>
+        <f t="shared" ref="J38:J39" si="5">E38+F38</f>
         <v>20</v>
       </c>
       <c r="K38">
@@ -4332,14 +4333,14 @@
         <v>1</v>
       </c>
       <c r="B39" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C39" t="str">
         <f t="shared" si="2"/>
         <v>Green#38</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E39">
         <v>20</v>
@@ -4351,13 +4352,13 @@
         <v>25</v>
       </c>
       <c r="H39" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I39">
         <v>4</v>
       </c>
       <c r="J39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>20</v>
       </c>
       <c r="K39">
@@ -4370,14 +4371,14 @@
         <v>1</v>
       </c>
       <c r="B40" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C40" t="str">
         <f t="shared" si="2"/>
         <v>Black#39</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E40">
         <v>2</v>
@@ -4389,11 +4390,11 @@
         <v>10</v>
       </c>
       <c r="J40">
-        <f>E40+F40</f>
+        <f t="shared" ref="J40:J49" si="6">E40+F40</f>
         <v>9</v>
       </c>
       <c r="K40">
-        <f>G40+I40</f>
+        <f t="shared" ref="K40:K49" si="7">G40+I40</f>
         <v>10</v>
       </c>
     </row>
@@ -4402,14 +4403,14 @@
         <v>1</v>
       </c>
       <c r="B41" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C41" t="str">
         <f t="shared" si="2"/>
         <v>Black#40</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E41">
         <v>0</v>
@@ -4421,11 +4422,11 @@
         <v>12</v>
       </c>
       <c r="J41">
-        <f>E41+F41</f>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="K41">
-        <f>G41+I41</f>
+        <f t="shared" si="7"/>
         <v>12</v>
       </c>
     </row>
@@ -4434,14 +4435,14 @@
         <v>1</v>
       </c>
       <c r="B42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C42" t="str">
         <f t="shared" si="2"/>
         <v>Black#41</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E42">
         <v>4</v>
@@ -4453,11 +4454,11 @@
         <v>12</v>
       </c>
       <c r="J42">
-        <f>E42+F42</f>
+        <f t="shared" si="6"/>
         <v>11</v>
       </c>
       <c r="K42">
-        <f>G42+I42</f>
+        <f t="shared" si="7"/>
         <v>12</v>
       </c>
     </row>
@@ -4466,14 +4467,14 @@
         <v>1</v>
       </c>
       <c r="B43" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C43" t="str">
         <f t="shared" si="2"/>
         <v>Black#42</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E43">
         <v>4</v>
@@ -4485,11 +4486,11 @@
         <v>14</v>
       </c>
       <c r="J43">
-        <f>E43+F43</f>
+        <f t="shared" si="6"/>
         <v>13</v>
       </c>
       <c r="K43">
-        <f>G43+I43</f>
+        <f t="shared" si="7"/>
         <v>14</v>
       </c>
     </row>
@@ -4498,14 +4499,14 @@
         <v>1</v>
       </c>
       <c r="B44" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C44" t="str">
         <f t="shared" si="2"/>
         <v>Black#43</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E44">
         <v>0</v>
@@ -4517,17 +4518,17 @@
         <v>13</v>
       </c>
       <c r="H44" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I44">
         <v>1</v>
       </c>
       <c r="J44">
-        <f>E44+F44</f>
+        <f t="shared" si="6"/>
         <v>11</v>
       </c>
       <c r="K44">
-        <f>G44+I44</f>
+        <f t="shared" si="7"/>
         <v>14</v>
       </c>
     </row>
@@ -4536,14 +4537,14 @@
         <v>1</v>
       </c>
       <c r="B45" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C45" t="str">
         <f t="shared" si="2"/>
         <v>Black#44</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E45">
         <v>1</v>
@@ -4555,11 +4556,11 @@
         <v>14</v>
       </c>
       <c r="J45">
-        <f>E45+F45</f>
+        <f t="shared" si="6"/>
         <v>11</v>
       </c>
       <c r="K45">
-        <f>G45+I45</f>
+        <f t="shared" si="7"/>
         <v>14</v>
       </c>
     </row>
@@ -4568,14 +4569,14 @@
         <v>1</v>
       </c>
       <c r="B46" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C46" t="str">
         <f t="shared" si="2"/>
         <v>Black#45</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E46">
         <v>0</v>
@@ -4587,17 +4588,17 @@
         <v>16</v>
       </c>
       <c r="H46" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I46">
         <v>2</v>
       </c>
       <c r="J46">
-        <f>E46+F46</f>
+        <f t="shared" si="6"/>
         <v>12</v>
       </c>
       <c r="K46">
-        <f>G46+I46</f>
+        <f t="shared" si="7"/>
         <v>18</v>
       </c>
     </row>
@@ -4606,14 +4607,14 @@
         <v>1</v>
       </c>
       <c r="B47" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C47" t="str">
         <f t="shared" si="2"/>
         <v>Black#46</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E47">
         <v>2</v>
@@ -4625,11 +4626,11 @@
         <v>15</v>
       </c>
       <c r="J47">
-        <f>E47+F47</f>
+        <f t="shared" si="6"/>
         <v>14</v>
       </c>
       <c r="K47">
-        <f>G47+I47</f>
+        <f t="shared" si="7"/>
         <v>15</v>
       </c>
     </row>
@@ -4638,14 +4639,14 @@
         <v>1</v>
       </c>
       <c r="B48" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C48" t="str">
         <f t="shared" si="2"/>
         <v>Black#47</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E48">
         <v>0</v>
@@ -4657,17 +4658,17 @@
         <v>19</v>
       </c>
       <c r="H48" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I48">
         <v>1</v>
       </c>
       <c r="J48">
-        <f>E48+F48</f>
+        <f t="shared" si="6"/>
         <v>14</v>
       </c>
       <c r="K48">
-        <f>G48+I48</f>
+        <f t="shared" si="7"/>
         <v>20</v>
       </c>
     </row>
@@ -4676,14 +4677,14 @@
         <v>1</v>
       </c>
       <c r="B49" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C49" t="str">
         <f t="shared" si="2"/>
         <v>Black#48</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E49">
         <v>0</v>
@@ -4695,17 +4696,17 @@
         <v>20</v>
       </c>
       <c r="H49" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I49">
         <v>1</v>
       </c>
       <c r="J49">
-        <f>E49+F49</f>
+        <f t="shared" si="6"/>
         <v>15</v>
       </c>
       <c r="K49">
-        <f>G49+I49</f>
+        <f t="shared" si="7"/>
         <v>21</v>
       </c>
     </row>
@@ -4714,14 +4715,14 @@
         <v>1</v>
       </c>
       <c r="B50" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C50" t="str">
         <f t="shared" si="2"/>
         <v>Black#49</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E50">
         <v>5</v>
@@ -4733,17 +4734,17 @@
         <v>20</v>
       </c>
       <c r="H50" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I50">
         <v>3</v>
       </c>
       <c r="J50">
-        <f t="shared" ref="J50:J51" si="4">E50+F50</f>
+        <f t="shared" ref="J50:J51" si="8">E50+F50</f>
         <v>22</v>
       </c>
       <c r="K50">
-        <f t="shared" ref="K50:K51" si="5">G50+I50</f>
+        <f t="shared" ref="K50:K51" si="9">G50+I50</f>
         <v>23</v>
       </c>
     </row>
@@ -4752,14 +4753,14 @@
         <v>1</v>
       </c>
       <c r="B51" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C51" t="str">
         <f t="shared" si="2"/>
         <v>Black#50</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E51">
         <v>0</v>
@@ -4771,17 +4772,17 @@
         <v>30</v>
       </c>
       <c r="H51" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I51">
         <v>4</v>
       </c>
       <c r="J51">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>20</v>
       </c>
       <c r="K51">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>34</v>
       </c>
     </row>

</xml_diff>